<commit_message>
check specify group same one T else F
</commit_message>
<xml_diff>
--- a/inputs/TestData1 (1).xlsx
+++ b/inputs/TestData1 (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\tranforming-dt-to-pnml\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF82641-26B6-41D7-9BED-06F86B58A670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AECA597-67C5-4805-8ACA-7D3A43EE1DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="10" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -246,24 +246,30 @@
   </si>
   <si>
     <t>&gt; </t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -272,7 +278,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -360,13 +366,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>211293</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>91352</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -700,26 +706,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2414180-2D19-4C86-B727-4046CC30FBFE}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.75" customWidth="1"/>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
-    <col min="4" max="4" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="14" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -763,7 +769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -789,7 +795,7 @@
         <v>50000</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="J2" t="s">
         <v>26</v>
@@ -801,13 +807,13 @@
         <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -827,19 +833,19 @@
         <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -862,16 +868,16 @@
         <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -888,10 +894,10 @@
         <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s">
         <v>27</v>
@@ -900,10 +906,10 @@
         <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -935,71 +941,103 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="N7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="N8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="M9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="K10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="K11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11" xr:uid="{33790ACD-A3AB-43D7-9383-48039305488A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E12" xr:uid="{33790ACD-A3AB-43D7-9383-48039305488A}">
       <formula1>"and, or"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1012,7 +1050,7 @@
           <x14:formula1>
             <xm:f>Configuration!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C14 G2:G11</xm:sqref>
+          <xm:sqref>G2:G12 C2:C15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1028,17 +1066,17 @@
       <selection activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="25" width="4.4140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="34" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="41" width="4.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="34" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="41" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1192,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1261,7 +1299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1475,7 +1513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1582,7 +1620,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1676,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1694,7 +1732,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1708,17 +1746,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBC4FF6-5597-48FD-A059-309A6CF0658C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="2.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="2.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1753,7 +1791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1776,7 +1814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1806,12 +1844,12 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="2.9140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1840,7 +1878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1857,7 +1895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1874,7 +1912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1896,7 +1934,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1910,21 +1948,21 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.75" customWidth="1"/>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
-    <col min="4" max="4" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.58203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1971,7 +2009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1984,7 +2022,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1997,7 +2035,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2010,7 +2048,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2023,7 +2061,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2036,7 +2074,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2049,7 +2087,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2062,7 +2100,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -2075,7 +2113,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2086,7 +2124,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2097,7 +2135,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2138,42 +2176,42 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -2191,13 +2229,13 @@
       <selection activeCell="E2" sqref="E2:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2253,7 +2291,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2309,7 +2347,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2365,7 +2403,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2421,7 +2459,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2444,7 +2482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2470,7 +2508,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2493,7 +2531,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2519,7 +2557,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -2554,13 +2592,13 @@
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2616,7 +2654,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2663,7 +2701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2710,7 +2748,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2757,7 +2795,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2780,7 +2818,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2797,7 +2835,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2814,7 +2852,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2850,13 +2888,13 @@
       <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2915,7 +2953,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2965,7 +3003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3015,7 +3053,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3067,7 +3105,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3087,7 +3125,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3107,7 +3145,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3140,13 +3178,13 @@
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3205,7 +3243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3255,7 +3293,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3305,7 +3343,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3356,7 +3394,7 @@
       </c>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3394,7 +3432,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3419,7 +3457,7 @@
       </c>
       <c r="U6" s="5"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3463,7 +3501,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22">
       <c r="P10" t="s">
         <v>35</v>
       </c>
@@ -3481,14 +3519,14 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="25" width="3.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="25" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3556,7 +3594,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3615,7 +3653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3674,7 +3712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3734,7 +3772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -3794,7 +3832,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3826,12 +3864,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
add wrtie txt file
</commit_message>
<xml_diff>
--- a/inputs/TestData1 (1).xlsx
+++ b/inputs/TestData1 (1).xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AECA597-67C5-4805-8ACA-7D3A43EE1DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566B9795-872A-417E-92E5-345E521B0FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId2"/>
-    <sheet name="Sheet1 (2)" sheetId="10" r:id="rId3"/>
-    <sheet name="Configuration" sheetId="9" r:id="rId4"/>
-    <sheet name="TestData1" sheetId="2" r:id="rId5"/>
-    <sheet name="TestData2" sheetId="4" r:id="rId6"/>
-    <sheet name="TestData3" sheetId="5" r:id="rId7"/>
-    <sheet name="TestData4" sheetId="6" r:id="rId8"/>
-    <sheet name="TestData5" sheetId="7" r:id="rId9"/>
-    <sheet name="TestData6" sheetId="8" r:id="rId10"/>
-    <sheet name="JSON1" sheetId="12" r:id="rId11"/>
-    <sheet name="JSON2" sheetId="13" r:id="rId12"/>
+    <sheet name="JSON2" sheetId="13" r:id="rId2"/>
+    <sheet name="JSON1" sheetId="12" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId4"/>
+    <sheet name="Sheet1 (2)" sheetId="10" r:id="rId5"/>
+    <sheet name="Configuration" sheetId="9" r:id="rId6"/>
+    <sheet name="TestData1" sheetId="2" r:id="rId7"/>
+    <sheet name="TestData2" sheetId="4" r:id="rId8"/>
+    <sheet name="TestData3" sheetId="5" r:id="rId9"/>
+    <sheet name="TestData4" sheetId="6" r:id="rId10"/>
+    <sheet name="TestData5" sheetId="7" r:id="rId11"/>
+    <sheet name="TestData6" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -709,7 +709,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -832,7 +832,7 @@
       <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="L3" t="s">
@@ -867,8 +867,8 @@
       <c r="K4" t="s">
         <v>27</v>
       </c>
-      <c r="L4" t="s">
-        <v>69</v>
+      <c r="L4" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>26</v>
@@ -960,8 +960,8 @@
       <c r="J7" t="s">
         <v>26</v>
       </c>
-      <c r="K7" t="s">
-        <v>26</v>
+      <c r="K7" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="L7" t="s">
         <v>27</v>
@@ -991,9 +991,6 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
       <c r="J9" t="s">
         <v>34</v>
       </c>
@@ -1004,6 +1001,9 @@
       </c>
       <c r="B10" t="s">
         <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
       </c>
       <c r="M10" t="s">
         <v>34</v>
@@ -1059,6 +1059,770 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978B0C4F-8962-4E22-BAE0-5F9F41A9C754}">
+  <dimension ref="A1:V10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N1">
+        <v>1.2</v>
+      </c>
+      <c r="O1">
+        <v>1.3</v>
+      </c>
+      <c r="P1">
+        <v>1.4</v>
+      </c>
+      <c r="Q1">
+        <v>2</v>
+      </c>
+      <c r="R1">
+        <v>3</v>
+      </c>
+      <c r="S1">
+        <v>4</v>
+      </c>
+      <c r="T1">
+        <v>5</v>
+      </c>
+      <c r="U1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="5"/>
+      <c r="Q6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9125E8-27F2-4A77-8908-B272A8A71459}">
+  <dimension ref="A1:Y8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="25" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K1" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="L1" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="M1" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="N1" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="O1" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="P1" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="R1" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="S1" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T1" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U1" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="V1" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="W1" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="X1" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D260BC-E31B-43E7-ACDD-617EA8AB0958}">
   <dimension ref="A1:AO8"/>
   <sheetViews>
@@ -1742,7 +2506,99 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9913B9C5-06AF-4E60-AFA0-F09BAD5545A7}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="2.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBC4FF6-5597-48FD-A059-309A6CF0658C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -1836,99 +2692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9913B9C5-06AF-4E60-AFA0-F09BAD5545A7}">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="9" max="9" width="2.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DB94E-6982-4057-B9D0-65A7CAB0CB94}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1940,7 +2704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B7733A-8005-4B55-A922-5DA93A8DDEEF}">
   <dimension ref="A1:O12"/>
   <sheetViews>
@@ -2168,7 +2932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A39C592-848D-4C48-AC9D-19ADD8348EFC}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -2221,7 +2985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7400FDEC-D497-4BBC-9902-8E4BE318F1B3}">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -2584,7 +3348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2148AE01-AB3B-4578-BB45-366590F09B83}">
   <dimension ref="A1:T8"/>
   <sheetViews>
@@ -2880,7 +3644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5203AA-6006-403D-B767-FB82C37B4A85}">
   <dimension ref="A1:X7"/>
   <sheetViews>
@@ -3168,768 +3932,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978B0C4F-8962-4E22-BAE0-5F9F41A9C754}">
-  <dimension ref="A1:V10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N1">
-        <v>1.2</v>
-      </c>
-      <c r="O1">
-        <v>1.3</v>
-      </c>
-      <c r="P1">
-        <v>1.4</v>
-      </c>
-      <c r="Q1">
-        <v>2</v>
-      </c>
-      <c r="R1">
-        <v>3</v>
-      </c>
-      <c r="S1">
-        <v>4</v>
-      </c>
-      <c r="T1">
-        <v>5</v>
-      </c>
-      <c r="U1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" s="5"/>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" t="s">
-        <v>34</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T7" t="s">
-        <v>34</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="P10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9125E8-27F2-4A77-8908-B272A8A71459}">
-  <dimension ref="A1:Y8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="25" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K1" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="L1" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="M1" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="N1" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="O1" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="P1" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="R1" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="S1" s="2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="T1" s="2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="U1" s="2">
-        <v>2.4</v>
-      </c>
-      <c r="V1" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="W1" s="2">
-        <v>2.6</v>
-      </c>
-      <c r="X1" s="2">
-        <v>2.7</v>
-      </c>
-      <c r="Y1" s="2">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug & modified write txt
</commit_message>
<xml_diff>
--- a/inputs/TestData1 (1).xlsx
+++ b/inputs/TestData1 (1).xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92476A4-282B-4DA1-ABF0-46BB21898C8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4854B9A-0428-4147-84ED-0D15B7A03855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="JSON2" sheetId="13" r:id="rId2"/>
-    <sheet name="JSON1" sheetId="12" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId4"/>
-    <sheet name="Sheet1 (2)" sheetId="10" r:id="rId5"/>
-    <sheet name="Configuration" sheetId="9" r:id="rId6"/>
-    <sheet name="TestData1" sheetId="2" r:id="rId7"/>
-    <sheet name="TestData2" sheetId="4" r:id="rId8"/>
-    <sheet name="TestData3" sheetId="5" r:id="rId9"/>
-    <sheet name="TestData4" sheetId="6" r:id="rId10"/>
-    <sheet name="TestData5" sheetId="7" r:id="rId11"/>
-    <sheet name="TestData6" sheetId="8" r:id="rId12"/>
+    <sheet name="Sheet1 (3)" sheetId="14" r:id="rId2"/>
+    <sheet name="JSON2" sheetId="13" r:id="rId3"/>
+    <sheet name="JSON1" sheetId="12" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId5"/>
+    <sheet name="Sheet1 (2)" sheetId="10" r:id="rId6"/>
+    <sheet name="Configuration" sheetId="9" r:id="rId7"/>
+    <sheet name="TestData1" sheetId="2" r:id="rId8"/>
+    <sheet name="TestData2" sheetId="4" r:id="rId9"/>
+    <sheet name="TestData3" sheetId="5" r:id="rId10"/>
+    <sheet name="TestData4" sheetId="6" r:id="rId11"/>
+    <sheet name="TestData5" sheetId="7" r:id="rId12"/>
+    <sheet name="TestData6" sheetId="8" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -273,6 +274,9 @@
   </si>
   <si>
     <t>Saraly</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -463,13 +467,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>163668</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>91352</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -495,6 +499,55 @@
         <a:xfrm>
           <a:off x="374650" y="2489200"/>
           <a:ext cx="11457143" cy="5780952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>163668</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>91352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1D81587-9B30-41D4-B6B9-82A0F7A8670F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="323850" y="3514725"/>
+          <a:ext cx="10164918" cy="6187352"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -803,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2414180-2D19-4C86-B727-4046CC30FBFE}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -958,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>73</v>
@@ -993,7 +1046,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="15"/>
@@ -1018,241 +1071,71 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A6" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>68</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A8" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A9" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L9" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" t="s">
-        <v>34</v>
-      </c>
-      <c r="L13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L10" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E14" xr:uid="{33790ACD-A3AB-43D7-9383-48039305488A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10" xr:uid="{33790ACD-A3AB-43D7-9383-48039305488A}">
       <formula1>"and, or"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1266,7 +1149,7 @@
           <x14:formula1>
             <xm:f>Configuration!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:C17 G10:G14</xm:sqref>
+          <xm:sqref>C6:C13 G6:G10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1275,6 +1158,296 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5203AA-6006-403D-B767-FB82C37B4A85}">
+  <dimension ref="A1:X7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N1">
+        <v>1.2</v>
+      </c>
+      <c r="O1">
+        <v>1.3</v>
+      </c>
+      <c r="P1">
+        <v>1.4</v>
+      </c>
+      <c r="Q1">
+        <v>2.1</v>
+      </c>
+      <c r="R1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T1">
+        <v>2.4</v>
+      </c>
+      <c r="U1">
+        <v>3.1</v>
+      </c>
+      <c r="V1">
+        <v>3.2</v>
+      </c>
+      <c r="W1">
+        <v>3.3</v>
+      </c>
+      <c r="X1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" t="s">
+        <v>34</v>
+      </c>
+      <c r="X7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978B0C4F-8962-4E22-BAE0-5F9F41A9C754}">
   <dimension ref="A1:V10"/>
   <sheetViews>
@@ -1615,7 +1788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9125E8-27F2-4A77-8908-B272A8A71459}">
   <dimension ref="A1:Y8"/>
   <sheetViews>
@@ -2038,7 +2211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D260BC-E31B-43E7-ACDD-617EA8AB0958}">
   <dimension ref="A1:AO8"/>
   <sheetViews>
@@ -2723,6 +2896,478 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA66153-CB74-458E-A35C-5C0F290B1C30}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A9" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E14" xr:uid="{9771E5DB-9069-4023-8495-C3AB518BE694}">
+      <formula1>"and, or"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3862D879-4B27-4888-AD28-8222CDC39AFC}">
+          <x14:formula1>
+            <xm:f>Configuration!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>C10:C17 G10:G14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9913B9C5-06AF-4E60-AFA0-F09BAD5545A7}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -2814,7 +3459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBC4FF6-5597-48FD-A059-309A6CF0658C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -2908,7 +3553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DB94E-6982-4057-B9D0-65A7CAB0CB94}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2920,7 +3565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B7733A-8005-4B55-A922-5DA93A8DDEEF}">
   <dimension ref="A1:O12"/>
   <sheetViews>
@@ -3148,7 +3793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A39C592-848D-4C48-AC9D-19ADD8348EFC}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -3201,7 +3846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7400FDEC-D497-4BBC-9902-8E4BE318F1B3}">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -3564,7 +4209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2148AE01-AB3B-4578-BB45-366590F09B83}">
   <dimension ref="A1:T8"/>
   <sheetViews>
@@ -3858,294 +4503,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5203AA-6006-403D-B767-FB82C37B4A85}">
-  <dimension ref="A1:X7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N1">
-        <v>1.2</v>
-      </c>
-      <c r="O1">
-        <v>1.3</v>
-      </c>
-      <c r="P1">
-        <v>1.4</v>
-      </c>
-      <c r="Q1">
-        <v>2.1</v>
-      </c>
-      <c r="R1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="S1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="T1">
-        <v>2.4</v>
-      </c>
-      <c r="U1">
-        <v>3.1</v>
-      </c>
-      <c r="V1">
-        <v>3.2</v>
-      </c>
-      <c r="W1">
-        <v>3.3</v>
-      </c>
-      <c r="X1">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W2" t="s">
-        <v>27</v>
-      </c>
-      <c r="X2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="M4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" t="s">
-        <v>26</v>
-      </c>
-      <c r="V4" t="s">
-        <v>26</v>
-      </c>
-      <c r="W4" t="s">
-        <v>26</v>
-      </c>
-      <c r="X4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="U7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V7" t="s">
-        <v>34</v>
-      </c>
-      <c r="W7" t="s">
-        <v>34</v>
-      </c>
-      <c r="X7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug condition one line
</commit_message>
<xml_diff>
--- a/inputs/TestData1 (1).xlsx
+++ b/inputs/TestData1 (1).xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4854B9A-0428-4147-84ED-0D15B7A03855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149C686F-DE0E-4E52-8AF1-55D32D82B9FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (3)" sheetId="14" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="14" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="JSON2" sheetId="13" r:id="rId3"/>
     <sheet name="JSON1" sheetId="12" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="11" r:id="rId5"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -240,9 +240,6 @@
     <t>and</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -267,16 +264,19 @@
     <t>B</t>
   </si>
   <si>
-    <t>or</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
-    <t>Saraly</t>
-  </si>
-  <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
 </sst>
 </file>
@@ -467,6 +467,55 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>163668</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>91352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1D81587-9B30-41D4-B6B9-82A0F7A8670F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="323850" y="3514725"/>
+          <a:ext cx="10164918" cy="6187352"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -499,55 +548,6 @@
         <a:xfrm>
           <a:off x="374650" y="2489200"/>
           <a:ext cx="11457143" cy="5780952"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>163668</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>91352</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1D81587-9B30-41D4-B6B9-82A0F7A8670F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="323850" y="3514725"/>
-          <a:ext cx="10164918" cy="6187352"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -855,11 +855,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2414180-2D19-4C86-B727-4046CC30FBFE}">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA66153-CB74-458E-A35C-5C0F290B1C30}">
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -880,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>38</v>
@@ -892,7 +892,7 @@
         <v>40</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>42</v>
@@ -924,20 +924,20 @@
         <v>4</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="12"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
         <v>26</v>
@@ -949,7 +949,7 @@
         <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
@@ -960,13 +960,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>72</v>
-      </c>
       <c r="D3" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="15"/>
@@ -996,29 +996,29 @@
         <v>10</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
         <v>73</v>
       </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
       <c r="J4" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>27</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>26</v>
@@ -1040,13 +1040,13 @@
         <v>36</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="15"/>
@@ -1068,74 +1068,206 @@
         <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
+      <c r="C7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>77</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L13" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10" xr:uid="{33790ACD-A3AB-43D7-9383-48039305488A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E13" xr:uid="{9771E5DB-9069-4023-8495-C3AB518BE694}">
       <formula1>"and, or"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1145,11 +1277,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7ED698B1-C7DC-49CF-AD16-F5AE762A202F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3862D879-4B27-4888-AD28-8222CDC39AFC}">
           <x14:formula1>
             <xm:f>Configuration!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C6:C13 G6:G10</xm:sqref>
+          <xm:sqref>C9:C16 G9:G13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2896,11 +3028,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA66153-CB74-458E-A35C-5C0F290B1C30}">
-  <dimension ref="A1:N14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2414180-2D19-4C86-B727-4046CC30FBFE}">
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2921,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>38</v>
@@ -2933,7 +3065,7 @@
         <v>40</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>42</v>
@@ -2965,20 +3097,20 @@
         <v>4</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="12"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
         <v>26</v>
@@ -2990,7 +3122,7 @@
         <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
@@ -3001,13 +3133,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>72</v>
-      </c>
       <c r="D3" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="15"/>
@@ -3037,29 +3169,29 @@
         <v>10</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
         <v>73</v>
       </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
       <c r="J4" t="s">
         <v>27</v>
       </c>
@@ -3067,7 +3199,7 @@
         <v>27</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>26</v>
@@ -3081,13 +3213,13 @@
         <v>36</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="15"/>
@@ -3109,243 +3241,74 @@
         <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A6" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>68</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A8" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A9" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L9" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" t="s">
-        <v>34</v>
-      </c>
-      <c r="L13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L10" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E14" xr:uid="{9771E5DB-9069-4023-8495-C3AB518BE694}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10" xr:uid="{33790ACD-A3AB-43D7-9383-48039305488A}">
       <formula1>"and, or"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3355,11 +3318,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3862D879-4B27-4888-AD28-8222CDC39AFC}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7ED698B1-C7DC-49CF-AD16-F5AE762A202F}">
           <x14:formula1>
             <xm:f>Configuration!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:C17 G10:G14</xm:sqref>
+          <xm:sqref>C6:C13 G6:G10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3434,7 +3397,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>43</v>
@@ -3519,7 +3482,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
fixed bug and unittest run testcase
</commit_message>
<xml_diff>
--- a/inputs/TestData1 (1).xlsx
+++ b/inputs/TestData1 (1).xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD43534-15C9-4400-8A99-EE93F39B5BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2157CE8-255D-48EE-8978-5DDE9467CDCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" xr2:uid="{59CE10C9-A357-44B2-B0C1-D4840FF3072D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (3)" sheetId="14" r:id="rId1"/>
-    <sheet name="Sheet1 (4)" sheetId="15" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="JSON2" sheetId="13" r:id="rId4"/>
-    <sheet name="JSON1" sheetId="12" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId6"/>
-    <sheet name="Sheet1 (2)" sheetId="10" r:id="rId7"/>
-    <sheet name="Configuration" sheetId="9" r:id="rId8"/>
-    <sheet name="TestData1" sheetId="2" r:id="rId9"/>
-    <sheet name="TestData2" sheetId="4" r:id="rId10"/>
-    <sheet name="TestData3" sheetId="5" r:id="rId11"/>
-    <sheet name="TestData4" sheetId="6" r:id="rId12"/>
-    <sheet name="TestData5" sheetId="7" r:id="rId13"/>
-    <sheet name="TestData6" sheetId="8" r:id="rId14"/>
+    <sheet name="Sheet1 (5)" sheetId="16" r:id="rId2"/>
+    <sheet name="Sheet1 (4)" sheetId="15" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="JSON2" sheetId="13" r:id="rId5"/>
+    <sheet name="JSON1" sheetId="12" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId7"/>
+    <sheet name="Sheet1 (2)" sheetId="10" r:id="rId8"/>
+    <sheet name="Configuration" sheetId="9" r:id="rId9"/>
+    <sheet name="TestData1" sheetId="2" r:id="rId10"/>
+    <sheet name="TestData2" sheetId="4" r:id="rId11"/>
+    <sheet name="TestData3" sheetId="5" r:id="rId12"/>
+    <sheet name="TestData4" sheetId="6" r:id="rId13"/>
+    <sheet name="TestData5" sheetId="7" r:id="rId14"/>
+    <sheet name="TestData6" sheetId="8" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -281,12 +282,6 @@
   </si>
   <si>
     <t>&lt; </t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
   </si>
   <si>
     <t>C11</t>
@@ -486,13 +481,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>554193</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>91352</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -530,6 +525,55 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>554193</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>91352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB7B075-58E5-42F6-9E5B-17B6BE3C54E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="323850" y="2505075"/>
+          <a:ext cx="10164918" cy="6187352"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -578,7 +622,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -924,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA66153-CB74-458E-A35C-5C0F290B1C30}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:N1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -943,7 +987,7 @@
     <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -973,255 +1017,115 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="13">
-        <v>15000</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="13">
-        <v>20000</v>
-      </c>
+      <c r="C2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
       <c r="I2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="14" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="16">
-        <v>15000</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="16">
-        <v>20000</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
       <c r="I3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="16">
-        <v>15000</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="16">
-        <v>50000</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="I4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A5" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="16">
-        <v>15000</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="16">
-        <v>50000</v>
-      </c>
-      <c r="I5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="16">
-        <v>15000</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="16">
-        <v>15000</v>
-      </c>
-      <c r="I6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A7" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="16">
-        <v>15000</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="16">
-        <v>50000</v>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
       </c>
       <c r="I7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A8" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="16">
-        <v>15000</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="16">
-        <v>50000</v>
-      </c>
-      <c r="I8" t="s">
-        <v>73</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E13" xr:uid="{9771E5DB-9069-4023-8495-C3AB518BE694}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E9" xr:uid="{9771E5DB-9069-4023-8495-C3AB518BE694}">
       <formula1>"and, or"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1235,7 +1139,7 @@
           <x14:formula1>
             <xm:f>Configuration!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C9:C16 G9:G13</xm:sqref>
+          <xm:sqref>C5:C12 G5:G9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1244,6 +1148,369 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7400FDEC-D497-4BBC-9902-8E4BE318F1B3}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="2">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2">
+        <v>2</v>
+      </c>
+      <c r="O1" s="2">
+        <v>3</v>
+      </c>
+      <c r="P1" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R1" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="S1" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="T1" s="2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>20000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2148AE01-AB3B-4578-BB45-366590F09B83}">
   <dimension ref="A1:T8"/>
   <sheetViews>
@@ -1539,7 +1806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5203AA-6006-403D-B767-FB82C37B4A85}">
   <dimension ref="A1:X7"/>
   <sheetViews>
@@ -1829,7 +2096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978B0C4F-8962-4E22-BAE0-5F9F41A9C754}">
   <dimension ref="A1:V10"/>
   <sheetViews>
@@ -2170,7 +2437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9125E8-27F2-4A77-8908-B272A8A71459}">
   <dimension ref="A1:Y8"/>
   <sheetViews>
@@ -2593,7 +2860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D260BC-E31B-43E7-ACDD-617EA8AB0958}">
   <dimension ref="A1:AO8"/>
   <sheetViews>
@@ -3278,11 +3545,215 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DCA263-02CC-43A0-96B3-CC2FD07009E9}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="16">
+        <v>15000</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="16">
+        <v>15000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A3" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="16">
+        <v>15000</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="16">
+        <v>50000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="16">
+        <v>15000</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="16">
+        <v>50000</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E9" xr:uid="{C9BD3837-3CC9-43AE-BBD2-0995C59E499C}">
+      <formula1>"and, or"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{61AA0D96-594A-41D6-8CBA-EA5702AECF1F}">
+          <x14:formula1>
+            <xm:f>Configuration!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C12 G5:G9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033392B2-32A9-482C-AE35-C63E402D20D9}">
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3711,7 +4182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2414180-2D19-4C86-B727-4046CC30FBFE}">
   <dimension ref="A1:N10"/>
   <sheetViews>
@@ -4014,7 +4485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9913B9C5-06AF-4E60-AFA0-F09BAD5545A7}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -4106,7 +4577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBC4FF6-5597-48FD-A059-309A6CF0658C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -4200,7 +4671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875DB94E-6982-4057-B9D0-65A7CAB0CB94}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4212,7 +4683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B7733A-8005-4B55-A922-5DA93A8DDEEF}">
   <dimension ref="A1:O12"/>
   <sheetViews>
@@ -4440,7 +4911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A39C592-848D-4C48-AC9D-19ADD8348EFC}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -4491,367 +4962,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7400FDEC-D497-4BBC-9902-8E4BE318F1B3}">
-  <dimension ref="A1:T9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="2">
-        <v>1</v>
-      </c>
-      <c r="N1" s="2">
-        <v>2</v>
-      </c>
-      <c r="O1" s="2">
-        <v>3</v>
-      </c>
-      <c r="P1" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="R1" s="2">
-        <v>5.2</v>
-      </c>
-      <c r="S1" s="2">
-        <v>6.1</v>
-      </c>
-      <c r="T1" s="2">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>20000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>